<commit_message>
agrega punto de pedido stock minimo y maximo
</commit_message>
<xml_diff>
--- a/src/assets/modelo_producto.xlsx
+++ b/src/assets/modelo_producto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t xml:space="preserve">precio_venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock_minimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock_maximo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">punto_de_pedido</t>
   </si>
 </sst>
 </file>
@@ -155,22 +164,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -188,6 +197,15 @@
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrega obs en listado de cheques
</commit_message>
<xml_diff>
--- a/src/assets/modelo_producto.xlsx
+++ b/src/assets/modelo_producto.xlsx
@@ -173,10 +173,14 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>